<commit_message>
Error: Cost iterative work in progress
</commit_message>
<xml_diff>
--- a/data/Properties_info.xlsx
+++ b/data/Properties_info.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fichtnergmbh-my.sharepoint.com/personal/flaizd_fis_fichtnergroup_com/Documents/Masterarbeit/Repository/Master-Thesis/OPTIMIZER/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{9736EA1E-F480-42C2-82BC-2A6E1E753514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC8F2D8C-A2F7-459A-91A0-AC020462C609}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{9736EA1E-F480-42C2-82BC-2A6E1E753514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCC76473-8AC1-49CD-957F-5635609E5497}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B51AB577-22E8-4532-B491-5B1100FF524D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,6 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -5586,16 +5591,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{854D6833-0145-46C8-8F71-1990252AD800}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>